<commit_message>
updating intermediaire de param_actu_IPP
</commit_message>
<xml_diff>
--- a/openfisca_france/param/Paramètres_OF_IPP.xlsx
+++ b/openfisca_france/param/Paramètres_OF_IPP.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="3885" windowWidth="18930" windowHeight="6060"/>
+    <workbookView xWindow="45" yWindow="3945" windowWidth="18930" windowHeight="6000"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -6432,18 +6432,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -6520,6 +6508,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6825,10 +6825,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J867"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A274" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A438" sqref="A438"/>
-      <selection pane="topRight" activeCell="C84" sqref="C84"/>
+      <selection pane="topRight" activeCell="F268" sqref="F268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6853,7 +6853,7 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="106" t="s">
+      <c r="C1" s="102" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -6879,7 +6879,7 @@
       <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="107"/>
+      <c r="C2" s="103"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -6915,7 +6915,7 @@
       <c r="B4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="108"/>
+      <c r="C4" s="104"/>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
@@ -6932,7 +6932,7 @@
       <c r="B5" s="9" t="s">
         <v>939</v>
       </c>
-      <c r="C5" s="108" t="s">
+      <c r="C5" s="104" t="s">
         <v>1722</v>
       </c>
       <c r="D5" s="8"/>
@@ -6951,7 +6951,7 @@
       <c r="B6" s="9" t="s">
         <v>1721</v>
       </c>
-      <c r="C6" s="108" t="s">
+      <c r="C6" s="104" t="s">
         <v>1722</v>
       </c>
       <c r="D6" s="8"/>
@@ -6969,7 +6969,7 @@
       <c r="B7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="109" t="s">
+      <c r="C7" s="105" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="11">
@@ -7006,7 +7006,7 @@
       <c r="B9" s="9" t="s">
         <v>939</v>
       </c>
-      <c r="C9" s="108" t="s">
+      <c r="C9" s="104" t="s">
         <v>1722</v>
       </c>
       <c r="D9" s="8"/>
@@ -7020,7 +7020,7 @@
       <c r="B10" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="C10" s="108" t="s">
+      <c r="C10" s="104" t="s">
         <v>1722</v>
       </c>
       <c r="D10" s="8"/>
@@ -7034,7 +7034,7 @@
       <c r="B11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="109" t="s">
+      <c r="C11" s="105" t="s">
         <v>22</v>
       </c>
       <c r="D11" s="11">
@@ -7070,7 +7070,7 @@
       <c r="B13" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="110" t="s">
+      <c r="C13" s="106" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="8"/>
@@ -7086,7 +7086,7 @@
       <c r="B14" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="111" t="s">
+      <c r="C14" s="107" t="s">
         <v>27</v>
       </c>
       <c r="D14" s="11"/>
@@ -7102,7 +7102,7 @@
       <c r="B15" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="112"/>
+      <c r="C15" s="108"/>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
       <c r="F15" s="6" t="s">
@@ -7118,7 +7118,7 @@
       <c r="B16" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="108"/>
+      <c r="C16" s="104"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
@@ -7132,7 +7132,7 @@
       <c r="B17" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="110" t="s">
+      <c r="C17" s="106" t="s">
         <v>27</v>
       </c>
       <c r="D17" s="8"/>
@@ -7146,7 +7146,7 @@
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
-      <c r="C18" s="110" t="s">
+      <c r="C18" s="106" t="s">
         <v>27</v>
       </c>
       <c r="D18" s="8"/>
@@ -7160,7 +7160,7 @@
       <c r="B19" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="109" t="s">
+      <c r="C19" s="105" t="s">
         <v>33</v>
       </c>
       <c r="D19" s="11"/>
@@ -7190,7 +7190,7 @@
       <c r="B21" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="110" t="s">
+      <c r="C21" s="106" t="s">
         <v>27</v>
       </c>
       <c r="D21" s="8"/>
@@ -7202,7 +7202,7 @@
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
-      <c r="C22" s="110" t="s">
+      <c r="C22" s="106" t="s">
         <v>27</v>
       </c>
       <c r="D22" s="8"/>
@@ -7216,7 +7216,7 @@
       <c r="B23" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="109" t="s">
+      <c r="C23" s="105" t="s">
         <v>36</v>
       </c>
       <c r="D23" s="11"/>
@@ -7234,7 +7234,7 @@
       <c r="B24" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="112"/>
+      <c r="C24" s="108"/>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
       <c r="F24" s="6" t="s">
@@ -7571,7 +7571,7 @@
       <c r="D43" s="17"/>
       <c r="E43" s="17"/>
       <c r="F43" s="17"/>
-      <c r="G43" s="95" t="s">
+      <c r="G43" s="124" t="s">
         <v>80</v>
       </c>
       <c r="H43" s="71"/>
@@ -7589,7 +7589,7 @@
       <c r="D44" s="17"/>
       <c r="E44" s="17"/>
       <c r="F44" s="17"/>
-      <c r="G44" s="96"/>
+      <c r="G44" s="125"/>
       <c r="H44" s="71"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -7599,7 +7599,7 @@
       <c r="B45" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C45" s="113"/>
+      <c r="C45" s="109"/>
       <c r="D45" s="22"/>
       <c r="E45" s="22"/>
       <c r="F45" s="22"/>
@@ -7613,7 +7613,7 @@
       <c r="B46" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="C46" s="114" t="s">
+      <c r="C46" s="110" t="s">
         <v>85</v>
       </c>
       <c r="D46" s="24"/>
@@ -7631,7 +7631,7 @@
       <c r="B47" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="C47" s="114" t="s">
+      <c r="C47" s="110" t="s">
         <v>85</v>
       </c>
       <c r="D47" s="24"/>
@@ -7649,7 +7649,7 @@
       <c r="B48" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="C48" s="115" t="s">
+      <c r="C48" s="111" t="s">
         <v>79</v>
       </c>
       <c r="D48" s="24"/>
@@ -7669,7 +7669,7 @@
       <c r="B49" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="C49" s="116"/>
+      <c r="C49" s="112"/>
       <c r="D49" s="29"/>
       <c r="E49" s="29"/>
       <c r="F49" s="29"/>
@@ -7683,7 +7683,7 @@
       <c r="B50" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="C50" s="117" t="s">
+      <c r="C50" s="113" t="s">
         <v>97</v>
       </c>
       <c r="D50" s="30"/>
@@ -7701,7 +7701,7 @@
       <c r="B51" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="C51" s="117" t="s">
+      <c r="C51" s="113" t="s">
         <v>101</v>
       </c>
       <c r="D51" s="30"/>
@@ -7719,7 +7719,7 @@
       <c r="B52" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="C52" s="117"/>
+      <c r="C52" s="113"/>
       <c r="D52" s="30"/>
       <c r="E52" s="30"/>
       <c r="F52" s="30" t="s">
@@ -7735,7 +7735,7 @@
       <c r="B53" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="C53" s="118" t="s">
+      <c r="C53" s="114" t="s">
         <v>107</v>
       </c>
       <c r="D53" s="32"/>
@@ -7753,7 +7753,7 @@
         <v>108</v>
       </c>
       <c r="B54" s="29"/>
-      <c r="C54" s="116"/>
+      <c r="C54" s="112"/>
       <c r="D54" s="29"/>
       <c r="E54" s="29"/>
       <c r="F54" s="29"/>
@@ -7776,7 +7776,7 @@
         <v>110</v>
       </c>
       <c r="B56" s="29"/>
-      <c r="C56" s="116"/>
+      <c r="C56" s="112"/>
       <c r="D56" s="29"/>
       <c r="E56" s="29"/>
       <c r="F56" s="29"/>
@@ -7792,7 +7792,7 @@
       <c r="B57" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="C57" s="112"/>
+      <c r="C57" s="108"/>
       <c r="D57" s="15"/>
       <c r="E57" s="15"/>
       <c r="F57" s="15"/>
@@ -7962,7 +7962,7 @@
       <c r="B66" s="75" t="s">
         <v>138</v>
       </c>
-      <c r="C66" s="121"/>
+      <c r="C66" s="117"/>
       <c r="D66" s="75"/>
       <c r="E66" s="75"/>
       <c r="F66" s="75"/>
@@ -8097,19 +8097,19 @@
       <c r="I72" s="43"/>
       <c r="J72" s="43"/>
     </row>
-    <row r="73" spans="1:10" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="99" t="s">
+    <row r="73" spans="1:10" s="97" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="95" t="s">
         <v>161</v>
       </c>
-      <c r="B73" s="99" t="s">
+      <c r="B73" s="95" t="s">
         <v>162</v>
       </c>
-      <c r="C73" s="119"/>
-      <c r="D73" s="99"/>
-      <c r="E73" s="99"/>
-      <c r="F73" s="99"/>
-      <c r="G73" s="100"/>
-      <c r="H73" s="100"/>
+      <c r="C73" s="115"/>
+      <c r="D73" s="95"/>
+      <c r="E73" s="95"/>
+      <c r="F73" s="95"/>
+      <c r="G73" s="96"/>
+      <c r="H73" s="96"/>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="17" t="s">
@@ -8494,7 +8494,7 @@
       <c r="B95" s="32" t="s">
         <v>1800</v>
       </c>
-      <c r="C95" s="120" t="s">
+      <c r="C95" s="116" t="s">
         <v>1801</v>
       </c>
       <c r="D95" s="50">
@@ -8751,7 +8751,7 @@
       <c r="B111" s="32" t="s">
         <v>1824</v>
       </c>
-      <c r="C111" s="120" t="s">
+      <c r="C111" s="116" t="s">
         <v>1801</v>
       </c>
       <c r="D111" s="32">
@@ -9042,10 +9042,10 @@
       <c r="H128" s="91"/>
     </row>
     <row r="129" spans="1:10" s="93" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="105" t="s">
+      <c r="A129" s="101" t="s">
         <v>1834</v>
       </c>
-      <c r="B129" s="102" t="s">
+      <c r="B129" s="98" t="s">
         <v>1835</v>
       </c>
       <c r="C129" s="92"/>
@@ -9132,10 +9132,10 @@
       <c r="H134" s="91"/>
     </row>
     <row r="135" spans="1:10" s="93" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="105" t="s">
+      <c r="A135" s="101" t="s">
         <v>1957</v>
       </c>
-      <c r="B135" s="102" t="s">
+      <c r="B135" s="98" t="s">
         <v>1846</v>
       </c>
       <c r="C135" s="92"/>
@@ -9183,10 +9183,10 @@
       <c r="H137" s="91"/>
     </row>
     <row r="138" spans="1:10" s="93" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="105" t="s">
+      <c r="A138" s="101" t="s">
         <v>1854</v>
       </c>
-      <c r="B138" s="102" t="s">
+      <c r="B138" s="98" t="s">
         <v>1855</v>
       </c>
       <c r="D138" s="50"/>
@@ -9230,10 +9230,10 @@
       <c r="H140" s="91"/>
     </row>
     <row r="141" spans="1:10" s="93" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="105" t="s">
+      <c r="A141" s="101" t="s">
         <v>1863</v>
       </c>
-      <c r="B141" s="102" t="s">
+      <c r="B141" s="98" t="s">
         <v>1864</v>
       </c>
       <c r="C141" s="92"/>
@@ -9269,7 +9269,7 @@
       <c r="A143" s="33" t="s">
         <v>1953</v>
       </c>
-      <c r="B143" s="102" t="s">
+      <c r="B143" s="98" t="s">
         <v>1869</v>
       </c>
       <c r="C143" s="43" t="s">
@@ -9322,7 +9322,7 @@
       <c r="B146" s="75" t="s">
         <v>1873</v>
       </c>
-      <c r="C146" s="121"/>
+      <c r="C146" s="117"/>
       <c r="D146" s="75"/>
       <c r="E146" s="75"/>
       <c r="F146" s="75"/>
@@ -9512,7 +9512,7 @@
       <c r="B156" s="33" t="s">
         <v>1721</v>
       </c>
-      <c r="C156" s="122" t="s">
+      <c r="C156" s="118" t="s">
         <v>1894</v>
       </c>
       <c r="D156" s="17"/>
@@ -9528,7 +9528,7 @@
       <c r="B157" s="33" t="s">
         <v>1736</v>
       </c>
-      <c r="C157" s="122" t="s">
+      <c r="C157" s="118" t="s">
         <v>1894</v>
       </c>
       <c r="D157" s="17"/>
@@ -9547,7 +9547,7 @@
         <v>1896</v>
       </c>
       <c r="C158" s="43"/>
-      <c r="D158" s="103"/>
+      <c r="D158" s="99"/>
       <c r="E158" s="17"/>
       <c r="F158" s="17" t="s">
         <v>1893</v>
@@ -9566,10 +9566,10 @@
       <c r="B159" s="33" t="s">
         <v>1721</v>
       </c>
-      <c r="C159" s="122" t="s">
+      <c r="C159" s="118" t="s">
         <v>1898</v>
       </c>
-      <c r="D159" s="103"/>
+      <c r="D159" s="99"/>
       <c r="E159" s="17"/>
       <c r="F159" s="17"/>
       <c r="G159" s="94"/>
@@ -9582,10 +9582,10 @@
       <c r="B160" s="33" t="s">
         <v>1736</v>
       </c>
-      <c r="C160" s="122" t="s">
+      <c r="C160" s="118" t="s">
         <v>1898</v>
       </c>
-      <c r="D160" s="103"/>
+      <c r="D160" s="99"/>
       <c r="E160" s="17"/>
       <c r="F160" s="17"/>
       <c r="G160" s="94"/>
@@ -9784,7 +9784,7 @@
       <c r="B171" s="17" t="s">
         <v>1920</v>
       </c>
-      <c r="C171" s="104" t="s">
+      <c r="C171" s="100" t="s">
         <v>1921</v>
       </c>
       <c r="D171" s="17"/>
@@ -9918,7 +9918,7 @@
       <c r="B178" s="33" t="s">
         <v>1721</v>
       </c>
-      <c r="C178" s="104" t="s">
+      <c r="C178" s="100" t="s">
         <v>1935</v>
       </c>
       <c r="D178" s="17"/>
@@ -9934,7 +9934,7 @@
       <c r="B179" s="33" t="s">
         <v>1736</v>
       </c>
-      <c r="C179" s="104" t="s">
+      <c r="C179" s="100" t="s">
         <v>1935</v>
       </c>
       <c r="D179" s="17"/>
@@ -10680,7 +10680,7 @@
         <v>1731</v>
       </c>
       <c r="B225" s="75"/>
-      <c r="C225" s="121"/>
+      <c r="C225" s="117"/>
       <c r="D225" s="75"/>
       <c r="E225" s="75"/>
       <c r="F225" s="75"/>
@@ -10737,7 +10737,7 @@
       <c r="B229" s="29" t="s">
         <v>175</v>
       </c>
-      <c r="C229" s="116"/>
+      <c r="C229" s="112"/>
       <c r="D229" s="29"/>
       <c r="E229" s="29"/>
       <c r="F229" s="29"/>
@@ -10751,7 +10751,7 @@
       <c r="B230" s="15" t="s">
         <v>1954</v>
       </c>
-      <c r="C230" s="112"/>
+      <c r="C230" s="108"/>
       <c r="D230" s="15"/>
       <c r="E230" s="15"/>
       <c r="F230" s="15" t="s">
@@ -10823,7 +10823,7 @@
       <c r="B234" s="35" t="s">
         <v>186</v>
       </c>
-      <c r="C234" s="123"/>
+      <c r="C234" s="119"/>
       <c r="D234" s="35"/>
       <c r="E234" s="35"/>
       <c r="F234" s="35"/>
@@ -10903,7 +10903,7 @@
       <c r="B239" s="35" t="s">
         <v>201</v>
       </c>
-      <c r="C239" s="124"/>
+      <c r="C239" s="120"/>
       <c r="D239" s="39"/>
       <c r="E239" s="39"/>
       <c r="F239" s="39"/>
@@ -10917,7 +10917,7 @@
       <c r="B240" s="30" t="s">
         <v>202</v>
       </c>
-      <c r="C240" s="117" t="s">
+      <c r="C240" s="113" t="s">
         <v>203</v>
       </c>
       <c r="D240" s="38"/>
@@ -10933,7 +10933,7 @@
       <c r="B241" s="38" t="s">
         <v>204</v>
       </c>
-      <c r="C241" s="117" t="s">
+      <c r="C241" s="113" t="s">
         <v>205</v>
       </c>
       <c r="D241" s="38"/>
@@ -10949,7 +10949,7 @@
       <c r="B242" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="C242" s="117" t="s">
+      <c r="C242" s="113" t="s">
         <v>207</v>
       </c>
       <c r="D242" s="38"/>
@@ -11097,7 +11097,7 @@
       <c r="B251" s="42" t="s">
         <v>232</v>
       </c>
-      <c r="C251" s="125" t="s">
+      <c r="C251" s="121" t="s">
         <v>233</v>
       </c>
       <c r="D251" s="38"/>
@@ -15515,7 +15515,7 @@
       <c r="E574" s="53">
         <v>2</v>
       </c>
-      <c r="H574" s="97" t="s">
+      <c r="H574" s="126" t="s">
         <v>996</v>
       </c>
     </row>
@@ -15533,7 +15533,7 @@
       <c r="E575" s="53">
         <v>2</v>
       </c>
-      <c r="H575" s="98"/>
+      <c r="H575" s="127"/>
     </row>
     <row r="576" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A576" s="41" t="s">
@@ -15633,7 +15633,7 @@
       <c r="B584" s="29" t="s">
         <v>1001</v>
       </c>
-      <c r="C584" s="116"/>
+      <c r="C584" s="112"/>
       <c r="D584" s="29"/>
       <c r="E584" s="29"/>
       <c r="F584" s="29"/>
@@ -17214,7 +17214,7 @@
       <c r="B705" s="29" t="s">
         <v>1309</v>
       </c>
-      <c r="C705" s="116"/>
+      <c r="C705" s="112"/>
       <c r="D705" s="29"/>
       <c r="E705" s="29"/>
       <c r="F705" s="29"/>
@@ -17284,7 +17284,7 @@
       <c r="B709" s="30" t="s">
         <v>1331</v>
       </c>
-      <c r="C709" s="126" t="s">
+      <c r="C709" s="122" t="s">
         <v>380</v>
       </c>
     </row>
@@ -17295,7 +17295,7 @@
       <c r="B710" s="30" t="s">
         <v>1332</v>
       </c>
-      <c r="C710" s="126" t="s">
+      <c r="C710" s="122" t="s">
         <v>27</v>
       </c>
       <c r="H710" s="73" t="s">
@@ -17309,7 +17309,7 @@
       <c r="B711" s="30" t="s">
         <v>1334</v>
       </c>
-      <c r="C711" s="126" t="s">
+      <c r="C711" s="122" t="s">
         <v>27</v>
       </c>
     </row>
@@ -17320,7 +17320,7 @@
       <c r="B712" s="30" t="s">
         <v>1333</v>
       </c>
-      <c r="C712" s="126" t="s">
+      <c r="C712" s="122" t="s">
         <v>380</v>
       </c>
     </row>
@@ -17339,7 +17339,7 @@
       <c r="B714" s="30" t="s">
         <v>1336</v>
       </c>
-      <c r="C714" s="126" t="s">
+      <c r="C714" s="122" t="s">
         <v>301</v>
       </c>
     </row>
@@ -17350,7 +17350,7 @@
       <c r="B715" s="30" t="s">
         <v>1337</v>
       </c>
-      <c r="C715" s="126" t="s">
+      <c r="C715" s="122" t="s">
         <v>301</v>
       </c>
     </row>
@@ -17361,7 +17361,7 @@
       <c r="B716" s="30" t="s">
         <v>1338</v>
       </c>
-      <c r="C716" s="126" t="s">
+      <c r="C716" s="122" t="s">
         <v>301</v>
       </c>
     </row>
@@ -17372,7 +17372,7 @@
       <c r="B717" s="30" t="s">
         <v>1339</v>
       </c>
-      <c r="C717" s="126" t="s">
+      <c r="C717" s="122" t="s">
         <v>301</v>
       </c>
     </row>
@@ -17383,7 +17383,7 @@
       <c r="B718" s="30" t="s">
         <v>1340</v>
       </c>
-      <c r="C718" s="126" t="s">
+      <c r="C718" s="122" t="s">
         <v>301</v>
       </c>
     </row>
@@ -17394,7 +17394,7 @@
       <c r="B719" s="30" t="s">
         <v>1341</v>
       </c>
-      <c r="C719" s="126" t="s">
+      <c r="C719" s="122" t="s">
         <v>301</v>
       </c>
     </row>
@@ -17405,7 +17405,7 @@
       <c r="B720" s="30" t="s">
         <v>1342</v>
       </c>
-      <c r="C720" s="126" t="s">
+      <c r="C720" s="122" t="s">
         <v>301</v>
       </c>
     </row>
@@ -17416,7 +17416,7 @@
       <c r="B721" s="30" t="s">
         <v>1343</v>
       </c>
-      <c r="C721" s="126" t="s">
+      <c r="C721" s="122" t="s">
         <v>301</v>
       </c>
     </row>
@@ -17427,7 +17427,7 @@
       <c r="B722" s="30" t="s">
         <v>1344</v>
       </c>
-      <c r="C722" s="126" t="s">
+      <c r="C722" s="122" t="s">
         <v>301</v>
       </c>
       <c r="D722" s="17"/>
@@ -17443,7 +17443,7 @@
       <c r="B723" s="30" t="s">
         <v>1345</v>
       </c>
-      <c r="C723" s="126" t="s">
+      <c r="C723" s="122" t="s">
         <v>301</v>
       </c>
     </row>
@@ -17454,7 +17454,7 @@
       <c r="B724" s="30" t="s">
         <v>1346</v>
       </c>
-      <c r="C724" s="126" t="s">
+      <c r="C724" s="122" t="s">
         <v>301</v>
       </c>
     </row>
@@ -17481,7 +17481,7 @@
       <c r="B726" s="30" t="s">
         <v>1360</v>
       </c>
-      <c r="C726" s="117"/>
+      <c r="C726" s="113"/>
       <c r="D726" s="30"/>
       <c r="E726" s="30"/>
       <c r="F726" s="30"/>
@@ -17541,7 +17541,7 @@
       <c r="B731" s="30" t="s">
         <v>1367</v>
       </c>
-      <c r="C731" s="117"/>
+      <c r="C731" s="113"/>
       <c r="D731" s="30"/>
       <c r="E731" s="30"/>
       <c r="F731" s="30"/>
@@ -17601,7 +17601,7 @@
       <c r="B736" s="30" t="s">
         <v>1380</v>
       </c>
-      <c r="C736" s="117"/>
+      <c r="C736" s="113"/>
       <c r="D736" s="30"/>
       <c r="E736" s="30"/>
       <c r="F736" s="30"/>
@@ -18085,7 +18085,7 @@
       <c r="B776" s="29" t="s">
         <v>1494</v>
       </c>
-      <c r="C776" s="116"/>
+      <c r="C776" s="112"/>
       <c r="D776" s="29"/>
       <c r="E776" s="29"/>
       <c r="F776" s="29"/>
@@ -18899,7 +18899,7 @@
       <c r="B838" s="29" t="s">
         <v>1664</v>
       </c>
-      <c r="C838" s="116"/>
+      <c r="C838" s="112"/>
       <c r="D838" s="29"/>
       <c r="E838" s="29"/>
       <c r="F838" s="28" t="s">
@@ -18955,7 +18955,7 @@
       <c r="B842" s="41" t="s">
         <v>1666</v>
       </c>
-      <c r="C842" s="127" t="s">
+      <c r="C842" s="123" t="s">
         <v>27</v>
       </c>
       <c r="D842" s="41"/>
@@ -18985,7 +18985,7 @@
       <c r="B844" s="53" t="s">
         <v>1708</v>
       </c>
-      <c r="C844" s="126" t="s">
+      <c r="C844" s="122" t="s">
         <v>27</v>
       </c>
     </row>
@@ -18996,7 +18996,7 @@
       <c r="B845" s="53" t="s">
         <v>1709</v>
       </c>
-      <c r="C845" s="126" t="s">
+      <c r="C845" s="122" t="s">
         <v>27</v>
       </c>
     </row>
@@ -19007,7 +19007,7 @@
       <c r="B846" s="53" t="s">
         <v>1710</v>
       </c>
-      <c r="C846" s="126" t="s">
+      <c r="C846" s="122" t="s">
         <v>27</v>
       </c>
     </row>
@@ -19018,7 +19018,7 @@
       <c r="B847" s="53" t="s">
         <v>1711</v>
       </c>
-      <c r="C847" s="126" t="s">
+      <c r="C847" s="122" t="s">
         <v>27</v>
       </c>
     </row>
@@ -19253,7 +19253,7 @@
       <c r="B866" s="29" t="s">
         <v>1714</v>
       </c>
-      <c r="C866" s="116"/>
+      <c r="C866" s="112"/>
       <c r="D866" s="29"/>
       <c r="E866" s="29"/>
       <c r="F866" s="28" t="s">

</xml_diff>

<commit_message>
Update OF IPP parameters
</commit_message>
<xml_diff>
--- a/openfisca_france/param/Paramètres_OF_IPP.xlsx
+++ b/openfisca_france/param/Paramètres_OF_IPP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="4065" windowWidth="18930" windowHeight="5880"/>
+    <workbookView xWindow="45" yWindow="4125" windowWidth="18930" windowHeight="5820"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -6853,10 +6853,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J875"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A164" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A843" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A438" sqref="A438"/>
-      <selection pane="topRight" activeCell="G192" sqref="G191:G192"/>
+      <selection pane="topRight" activeCell="C867" sqref="C867"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>